<commit_message>
add (Hul, 2012) and (Lijnen, 2007) data to vessel size and vessel density
</commit_message>
<xml_diff>
--- a/data/vessel_parameters.xlsx
+++ b/data/vessel_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EBF652D-EB5C-9543-BADE-A1706AF7C7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A054559-A988-6B4A-88E7-0834F60DFA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7840" windowWidth="29400" windowHeight="8360" activeTab="5" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
+    <workbookView xWindow="10060" yWindow="1580" windowWidth="29400" windowHeight="8360" activeTab="2" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel size (adipose)" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="CBM (retina)" sheetId="6" r:id="rId5"/>
     <sheet name="CBM (muscle)" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
   <si>
     <t>Reference</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>Lash et al., 1989 (18 wk.)</t>
+  </si>
+  <si>
+    <t>Hul et al., 2012</t>
+  </si>
+  <si>
+    <t>Lijnen et al., 2007</t>
   </si>
 </sst>
 </file>
@@ -192,8 +198,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9345D645-B0C0-EB46-8246-BA16416A932D}" name="Table1" displayName="Table1" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6" xr:uid="{9345D645-B0C0-EB46-8246-BA16416A932D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9345D645-B0C0-EB46-8246-BA16416A932D}" name="Table1" displayName="Table1" ref="A1:E8" totalsRowShown="0">
+  <autoFilter ref="A1:E8" xr:uid="{9345D645-B0C0-EB46-8246-BA16416A932D}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B6B21CB4-3BF8-CA4F-B6D1-667B8F16ACAD}" name="Reference"/>
     <tableColumn id="2" xr3:uid="{AD7C98EC-957C-DD40-BE11-28117E12F20A}" name="Lean_Average"/>
@@ -218,8 +224,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B76B723-8419-4C40-A482-C96E89DAF113}" name="Table13" displayName="Table13" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6" xr:uid="{2B76B723-8419-4C40-A482-C96E89DAF113}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B76B723-8419-4C40-A482-C96E89DAF113}" name="Table13" displayName="Table13" ref="A1:E8" totalsRowShown="0">
+  <autoFilter ref="A1:E8" xr:uid="{2B76B723-8419-4C40-A482-C96E89DAF113}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{628F8917-DB36-EB45-9027-3E96F8944A3A}" name="Reference"/>
     <tableColumn id="2" xr3:uid="{6CF8D7DE-ECB1-3141-83D3-8C52A6C13012}" name="Lean_Average"/>
@@ -568,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C67B71-C5D5-0C49-8DD9-33AB5A060F17}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -670,6 +676,34 @@
       </c>
       <c r="E6">
         <v>3.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>59</v>
+      </c>
+      <c r="C7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D7">
+        <v>49</v>
+      </c>
+      <c r="E7">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>108</v>
+      </c>
+      <c r="E8">
+        <v>7.7</v>
       </c>
     </row>
   </sheetData>
@@ -803,10 +837,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB9AA12-EEBC-1B4E-A018-35116729BAA8}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -906,6 +940,34 @@
       </c>
       <c r="E6">
         <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>740</v>
+      </c>
+      <c r="C7">
+        <v>96</v>
+      </c>
+      <c r="D7">
+        <v>400</v>
+      </c>
+      <c r="E7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>238</v>
+      </c>
+      <c r="E8">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1098,7 +1160,7 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E4" si="0">C3/SQRT(D3)</f>
+        <f t="shared" ref="E3" si="0">C3/SQRT(D3)</f>
         <v>6.6821590822128734</v>
       </c>
     </row>
@@ -1126,7 +1188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3778E71-8C6C-F642-91B5-016CE0E76C01}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix typo in vessel size sheet
</commit_message>
<xml_diff>
--- a/data/vessel_parameters.xlsx
+++ b/data/vessel_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A054559-A988-6B4A-88E7-0834F60DFA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8888AFEB-4D0A-CA44-B27D-41277F9B674C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10060" yWindow="1580" windowWidth="29400" windowHeight="8360" activeTab="2" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="8360" activeTab="3" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel size (adipose)" sheetId="2" r:id="rId1"/>
@@ -839,7 +839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB9AA12-EEBC-1B4E-A018-35116729BAA8}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -982,7 +982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{948AD4BD-5858-C44D-9CCF-6A7A80C70BF7}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1103,7 +1103,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1133,7 +1133,7 @@
         <v>26</v>
       </c>
       <c r="B2">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C2">
         <v>13</v>
@@ -1189,7 +1189,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
1. Edit reference name `Hul et al., 2012` -> `Van Hul et al., 2012` 2. Edit reference name `Lijnen, 2003` -> `Lijnen et al., 2003` 3. Delete `Koyama, 2017` from vessel size (too large)
</commit_message>
<xml_diff>
--- a/data/vessel_parameters.xlsx
+++ b/data/vessel_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8888AFEB-4D0A-CA44-B27D-41277F9B674C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9781209-9424-7343-97CD-C3F9C3ADA9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="8360" activeTab="3" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16680" firstSheet="1" activeTab="1" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel size (adipose)" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>Reference</t>
   </si>
@@ -55,9 +55,6 @@
     <t>SD</t>
   </si>
   <si>
-    <t>Lijnen, 2003</t>
-  </si>
-  <si>
     <t>Lean_Average</t>
   </si>
   <si>
@@ -139,10 +136,13 @@
     <t>Lash et al., 1989 (18 wk.)</t>
   </si>
   <si>
-    <t>Hul et al., 2012</t>
-  </si>
-  <si>
     <t>Lijnen et al., 2007</t>
+  </si>
+  <si>
+    <t>Van Hul et al., 2012</t>
+  </si>
+  <si>
+    <t>Lijnen et al., 2003</t>
   </si>
 </sst>
 </file>
@@ -212,8 +212,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{44B5E82D-DA16-C541-862F-3E86577D1164}" name="Table3" displayName="Table3" ref="A1:C9" totalsRowShown="0">
-  <autoFilter ref="A1:C9" xr:uid="{44B5E82D-DA16-C541-862F-3E86577D1164}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{44B5E82D-DA16-C541-862F-3E86577D1164}" name="Table3" displayName="Table3" ref="A1:C8" totalsRowShown="0">
+  <autoFilter ref="A1:C8" xr:uid="{44B5E82D-DA16-C541-862F-3E86577D1164}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A2B929B1-1D90-9E49-83F2-D169F4B69A23}" name="Reference"/>
     <tableColumn id="2" xr3:uid="{D3E2220D-5C65-6942-A58D-E3C127B02764}" name="Average"/>
@@ -577,7 +577,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -593,21 +593,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>27</v>
@@ -624,7 +624,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>49</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>74</v>
@@ -658,7 +658,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>47</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>76</v>
@@ -697,7 +697,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8">
         <v>108</v>
@@ -716,10 +716,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B85283-A6CE-8E41-B263-5F254FE23441}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -741,7 +741,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>53</v>
@@ -752,7 +752,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>130</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>84.95</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>86.59</v>
@@ -785,7 +785,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>134.80000000000001</v>
@@ -796,7 +796,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>93.3</v>
@@ -807,24 +807,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>113.1</v>
       </c>
       <c r="C8">
         <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9">
-        <v>37.9</v>
-      </c>
-      <c r="C9">
-        <v>0.78500000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +829,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -857,21 +846,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>370</v>
@@ -888,7 +877,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>790</v>
@@ -905,7 +894,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>280</v>
@@ -922,7 +911,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>120</v>
@@ -933,7 +922,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>210</v>
@@ -961,7 +950,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8">
         <v>238</v>
@@ -982,7 +971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{948AD4BD-5858-C44D-9CCF-6A7A80C70BF7}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1004,7 +993,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>125.79</v>
@@ -1015,7 +1004,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>19.45</v>
@@ -1026,7 +1015,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>19.13</v>
@@ -1037,7 +1026,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>17.64</v>
@@ -1048,7 +1037,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>70.62</v>
@@ -1059,7 +1048,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>31.87</v>
@@ -1070,7 +1059,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>29.65</v>
@@ -1081,7 +1070,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <v>147.74</v>
@@ -1103,7 +1092,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1122,7 +1111,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1130,7 +1119,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>59</v>
@@ -1148,7 +1137,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>92.87</v>
@@ -1166,7 +1155,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>89</v>
@@ -1189,7 +1178,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1208,7 +1197,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1216,7 +1205,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>73</v>
@@ -1234,7 +1223,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>76.75</v>
@@ -1252,7 +1241,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>62</v>
@@ -1270,7 +1259,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>56</v>

</xml_diff>

<commit_message>
exclude (Koyama, 2017) from `Vessel density (tumor)` sheet
</commit_message>
<xml_diff>
--- a/data/vessel_parameters.xlsx
+++ b/data/vessel_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9781209-9424-7343-97CD-C3F9C3ADA9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888F0C8F-3EC4-6D4F-9AC6-5942F0FF18AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16680" firstSheet="1" activeTab="1" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16680" firstSheet="1" activeTab="3" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel size (adipose)" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>Reference</t>
   </si>
@@ -101,9 +101,6 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>Koyama et al., 2017</t>
   </si>
   <si>
     <t>Fernandez-Rodrigues et al., 2016</t>
@@ -238,8 +235,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}" name="Table4" displayName="Table4" ref="A1:C9" totalsRowShown="0">
-  <autoFilter ref="A1:C9" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}" name="Table4" displayName="Table4" ref="A1:C8" totalsRowShown="0">
+  <autoFilter ref="A1:C8" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0F912B10-92FC-BC4D-9A6F-BC8B503601C9}" name="Reference"/>
     <tableColumn id="2" xr3:uid="{06728376-F009-934F-B3F0-B125D2C41224}" name="Average"/>
@@ -658,7 +655,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5">
         <v>47</v>
@@ -680,7 +677,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>59</v>
@@ -697,7 +694,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8">
         <v>108</v>
@@ -718,7 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B85283-A6CE-8E41-B263-5F254FE23441}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -911,7 +908,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5">
         <v>120</v>
@@ -933,7 +930,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>740</v>
@@ -950,7 +947,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8">
         <v>238</v>
@@ -969,10 +966,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{948AD4BD-5858-C44D-9CCF-6A7A80C70BF7}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -993,46 +990,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>125.79</v>
+        <v>19.45</v>
       </c>
       <c r="C2">
-        <v>5.2</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B3">
-        <v>19.45</v>
+        <v>19.13</v>
       </c>
       <c r="C3">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4">
-        <v>19.13</v>
+        <v>17.64</v>
       </c>
       <c r="C4">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5">
-        <v>17.64</v>
+        <v>70.62</v>
       </c>
       <c r="C5">
-        <v>2.4</v>
+        <v>9.74</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1040,10 +1037,10 @@
         <v>21</v>
       </c>
       <c r="B6">
-        <v>70.62</v>
+        <v>31.87</v>
       </c>
       <c r="C6">
-        <v>9.74</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1051,10 +1048,10 @@
         <v>22</v>
       </c>
       <c r="B7">
-        <v>31.87</v>
+        <v>29.65</v>
       </c>
       <c r="C7">
-        <v>5.8</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1062,20 +1059,9 @@
         <v>23</v>
       </c>
       <c r="B8">
-        <v>29.65</v>
+        <v>147.74</v>
       </c>
       <c r="C8">
-        <v>2.81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9">
-        <v>147.74</v>
-      </c>
-      <c r="C9">
         <v>17.899999999999999</v>
       </c>
     </row>
@@ -1119,7 +1105,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>59</v>
@@ -1137,7 +1123,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>92.87</v>
@@ -1155,7 +1141,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>89</v>
@@ -1205,7 +1191,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>73</v>
@@ -1223,7 +1209,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>76.75</v>
@@ -1241,7 +1227,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>62</v>
@@ -1259,7 +1245,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>56</v>

</xml_diff>

<commit_message>
edit vessel density in (Lijnen, 2006) and (Goel, 2013) to `Vessel density (tumor)` sheet
</commit_message>
<xml_diff>
--- a/data/vessel_parameters.xlsx
+++ b/data/vessel_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65050120-1407-0C47-BF52-E1DF81277DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8698690B-677F-EC43-B6C8-F2F51237808F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17880" yWindow="740" windowWidth="14700" windowHeight="16680" firstSheet="2" activeTab="5" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
+    <workbookView xWindow="0" yWindow="9080" windowWidth="19280" windowHeight="8360" activeTab="3" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel size (adipose)" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
   <si>
     <t>Reference</t>
   </si>
@@ -235,8 +235,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}" name="Table4" displayName="Table4" ref="A1:C8" totalsRowShown="0">
-  <autoFilter ref="A1:C8" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}" name="Table4" displayName="Table4" ref="A1:C10" totalsRowShown="0">
+  <autoFilter ref="A1:C10" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0F912B10-92FC-BC4D-9A6F-BC8B503601C9}" name="Reference"/>
     <tableColumn id="2" xr3:uid="{06728376-F009-934F-B3F0-B125D2C41224}" name="Average"/>
@@ -716,7 +716,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A4" sqref="A4:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -826,7 +826,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -863,7 +863,7 @@
         <v>370</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D2">
         <v>290</v>
@@ -966,10 +966,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{948AD4BD-5858-C44D-9CCF-6A7A80C70BF7}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1063,6 +1063,28 @@
       </c>
       <c r="C8">
         <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>292.45</v>
+      </c>
+      <c r="C9">
+        <v>28.64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>211.93</v>
+      </c>
+      <c r="C10">
+        <v>25.6</v>
       </c>
     </row>
   </sheetData>
@@ -1163,7 +1185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3778E71-8C6C-F642-91B5-016CE0E76C01}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
edit vessel size SE in (Tufto & Rofstad, 1999)
</commit_message>
<xml_diff>
--- a/data/vessel_parameters.xlsx
+++ b/data/vessel_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61110530-BB3B-764A-97DA-76DFA3B826F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04C595F-611B-AF49-8B6B-1739FC59FC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9080" windowWidth="19280" windowHeight="8360" activeTab="3" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel size (adipose)" sheetId="2" r:id="rId1"/>
@@ -574,7 +574,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -715,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B85283-A6CE-8E41-B263-5F254FE23441}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,7 +788,7 @@
         <v>134.80000000000001</v>
       </c>
       <c r="C6">
-        <v>10.6</v>
+        <v>8.32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -799,7 +799,7 @@
         <v>93.3</v>
       </c>
       <c r="C7">
-        <v>5.4</v>
+        <v>4.2300000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -810,7 +810,7 @@
         <v>113.1</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>5.51</v>
       </c>
     </row>
   </sheetData>
@@ -826,7 +826,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{948AD4BD-5858-C44D-9CCF-6A7A80C70BF7}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add CBM thickness in kidney
</commit_message>
<xml_diff>
--- a/data/vessel_parameters.xlsx
+++ b/data/vessel_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04C595F-611B-AF49-8B6B-1739FC59FC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E252E16B-CB35-FC45-BA7F-68EBDE041694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" firstSheet="3" activeTab="6" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel size (adipose)" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Vessel density (tumor)" sheetId="5" r:id="rId4"/>
     <sheet name="CBM (retina)" sheetId="6" r:id="rId5"/>
     <sheet name="CBM (muscle)" sheetId="7" r:id="rId6"/>
+    <sheet name="CBM (kidney)" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>Reference</t>
   </si>
@@ -140,6 +141,21 @@
   </si>
   <si>
     <t>Lijnen et al., 2003</t>
+  </si>
+  <si>
+    <t>Chang et al., 2012</t>
+  </si>
+  <si>
+    <t>Gambaro et al., 1992</t>
+  </si>
+  <si>
+    <t>Yagihashi, 1978 (6 month-old rats)</t>
+  </si>
+  <si>
+    <t>Yagihashi, 1978 (7 month-old rats)</t>
+  </si>
+  <si>
+    <t>Ireland et al., 1977</t>
   </si>
 </sst>
 </file>
@@ -269,6 +285,20 @@
     <tableColumn id="3" xr3:uid="{6E424A94-9406-5642-AD5C-0CBDD4AC95C8}" name="SD"/>
     <tableColumn id="4" xr3:uid="{6BC8F42A-61E2-AD4B-B9FD-15E2C1CF3327}" name="N"/>
     <tableColumn id="5" xr3:uid="{4901A108-E9A6-5E40-958F-B53E470CD03B}" name="SE"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{75009760-B3AA-0840-930F-D2CDF2C281B5}" name="Table58" displayName="Table58" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{75009760-B3AA-0840-930F-D2CDF2C281B5}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{F663CDD2-D3B9-904E-B285-49DAC8870978}" name="Reference"/>
+    <tableColumn id="2" xr3:uid="{96EE9805-BA6F-4441-8B97-1F18D839E4E5}" name="Average"/>
+    <tableColumn id="3" xr3:uid="{1F3FB073-7DBD-FF4C-B602-EEA5E6607750}" name="SD"/>
+    <tableColumn id="4" xr3:uid="{F5A9B8A8-2E67-A64F-A24E-5EAB6675757E}" name="N"/>
+    <tableColumn id="5" xr3:uid="{88A4B682-E733-934A-8C16-16DEC42C6D52}" name="SE"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -715,7 +745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B85283-A6CE-8E41-B263-5F254FE23441}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1100,7 +1130,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1281,4 +1311,133 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8638496-EB20-CE45-9016-2212A07E7085}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>178.16</v>
+      </c>
+      <c r="C2">
+        <v>35.61</v>
+      </c>
+      <c r="D2">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <f>C2/SQRT(D2)</f>
+        <v>8.1694942831307031</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>224.2</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>27.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>235.57</v>
+      </c>
+      <c r="E4">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>160.5</v>
+      </c>
+      <c r="C5">
+        <v>3.8</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <f>C5/SQRT(D5)</f>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6">
+        <v>184.6</v>
+      </c>
+      <c r="C6">
+        <v>6.5</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f>C6/SQRT(D6)</f>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7">
+        <v>305</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
edit reference names of tumor vessel parameters so that it contains mice strain and tumor cell types
</commit_message>
<xml_diff>
--- a/data/vessel_parameters.xlsx
+++ b/data/vessel_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E252E16B-CB35-FC45-BA7F-68EBDE041694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED111FFC-78EB-524D-8B75-9761C8307826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" firstSheet="3" activeTab="6" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="3" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel size (adipose)" sheetId="2" r:id="rId1"/>
@@ -80,42 +80,9 @@
     <t>Maquoi et al., 2003</t>
   </si>
   <si>
-    <t>Tufto &amp; Rofstad, 1999 (D-12 cell)</t>
-  </si>
-  <si>
-    <t>Mesquita et al., 2012 (C3H mice)</t>
-  </si>
-  <si>
-    <t>Mesquita et al., 2012 (Nude mice)</t>
-  </si>
-  <si>
-    <t>Goel et al., 2013 (Nude mice)</t>
-  </si>
-  <si>
-    <t>Goel et al., 2013 (C57BL6/J mice)</t>
-  </si>
-  <si>
-    <t>Tufto &amp; Rofstad, 1999 (R-18 cell)</t>
-  </si>
-  <si>
-    <t>Tufto &amp; Rofstad, 1999 (U-25 cell)</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
-    <t>Fernandez-Rodrigues et al., 2016</t>
-  </si>
-  <si>
-    <t>Kostourou et al., 2013 (B16F0 cell)</t>
-  </si>
-  <si>
-    <t>Kostourou et al., 2013 (CMT19T cell)</t>
-  </si>
-  <si>
-    <t>Jones et al., 2013</t>
-  </si>
-  <si>
     <t>Cuthbertson &amp; Mandel, 1986</t>
   </si>
   <si>
@@ -156,6 +123,39 @@
   </si>
   <si>
     <t>Ireland et al., 1977</t>
+  </si>
+  <si>
+    <t>Mesquita et al., 2012 (C3H mice &amp; fibrosarcoma)</t>
+  </si>
+  <si>
+    <t>Mesquita et al., 2012 (Nude mice &amp; fibrosarcoma)</t>
+  </si>
+  <si>
+    <t>Tufto &amp; Rofstad, 1999 (Balb/c nu/nu &amp; D-12 cell)</t>
+  </si>
+  <si>
+    <t>Tufto &amp; Rofstad, 1999 (Balb/c nu/nu &amp; R-18 cell)</t>
+  </si>
+  <si>
+    <t>Tufto &amp; Rofstad, 1999 (Balb/c nu/nu &amp; U-25 cell)</t>
+  </si>
+  <si>
+    <t>Fernandez-Rodrigues et al., 2016 (C57Bl/6 &amp; B16F1)</t>
+  </si>
+  <si>
+    <t>Kostourou et al., 2013 (C57BL6/129 &amp; B16F0 cell)</t>
+  </si>
+  <si>
+    <t>Kostourou et al., 2013 (C57BL6/129 &amp; CMT19T cell)</t>
+  </si>
+  <si>
+    <t>Jones et al., 2013 (C57BL6 &amp; LLC cell)</t>
+  </si>
+  <si>
+    <t>Goel et al., 2013 (Nude &amp; 4T1 primary tumor)</t>
+  </si>
+  <si>
+    <t>Goel et al., 2013 (C57BL6/J &amp; E0771 tumor)</t>
   </si>
 </sst>
 </file>
@@ -685,7 +685,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>47</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>59</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <v>108</v>
@@ -746,12 +746,12 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.1640625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -768,7 +768,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>53</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>130</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>84.95</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>86.59</v>
@@ -812,7 +812,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>134.80000000000001</v>
@@ -823,7 +823,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>93.3</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <v>113.1</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>120</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>740</v>
@@ -977,7 +977,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <v>238</v>
@@ -998,13 +998,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{948AD4BD-5858-C44D-9CCF-6A7A80C70BF7}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1020,7 +1020,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>19.45</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>19.13</v>
@@ -1042,7 +1042,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>17.64</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>70.62</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>31.87</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>29.65</v>
@@ -1086,7 +1086,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>147.74</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B9">
         <v>292.45</v>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>211.93</v>
@@ -1149,7 +1149,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>59</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>92.87</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>89</v>
@@ -1235,7 +1235,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>73</v>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>76.75</v>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>61.87</v>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>55.67</v>
@@ -1317,7 +1317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8638496-EB20-CE45-9016-2212A07E7085}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1338,7 +1338,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1346,7 +1346,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>178.16</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>224.2</v>
@@ -1378,7 +1378,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>235.57</v>
@@ -1389,7 +1389,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>160.5</v>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>184.6</v>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>305</v>

</xml_diff>

<commit_message>
delete "mice" from reference name in `Vessel size (tumor)` Sheet
</commit_message>
<xml_diff>
--- a/data/vessel_parameters.xlsx
+++ b/data/vessel_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED111FFC-78EB-524D-8B75-9761C8307826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B029243E-C004-8044-B5AA-D9A2B4CE0D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="3" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
   </bookViews>
@@ -125,12 +125,6 @@
     <t>Ireland et al., 1977</t>
   </si>
   <si>
-    <t>Mesquita et al., 2012 (C3H mice &amp; fibrosarcoma)</t>
-  </si>
-  <si>
-    <t>Mesquita et al., 2012 (Nude mice &amp; fibrosarcoma)</t>
-  </si>
-  <si>
     <t>Tufto &amp; Rofstad, 1999 (Balb/c nu/nu &amp; D-12 cell)</t>
   </si>
   <si>
@@ -156,6 +150,12 @@
   </si>
   <si>
     <t>Goel et al., 2013 (C57BL6/J &amp; E0771 tumor)</t>
+  </si>
+  <si>
+    <t>Mesquita et al., 2012 (C3H &amp; fibrosarcoma)</t>
+  </si>
+  <si>
+    <t>Mesquita et al., 2012 (Nude &amp; fibrosarcoma)</t>
   </si>
 </sst>
 </file>
@@ -746,7 +746,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,7 +768,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>53</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>130</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4">
         <v>84.95</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <v>86.59</v>
@@ -812,7 +812,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>134.80000000000001</v>
@@ -823,7 +823,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7">
         <v>93.3</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>113.1</v>
@@ -999,7 +999,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1020,7 +1020,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>19.45</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>19.13</v>
@@ -1042,7 +1042,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>17.64</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>70.62</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>31.87</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>29.65</v>
@@ -1086,7 +1086,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>147.74</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>292.45</v>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>211.93</v>

</xml_diff>

<commit_message>
change the reference name `Ireland et al., 1977` to `Fox et al., 1977`
</commit_message>
<xml_diff>
--- a/data/vessel_parameters.xlsx
+++ b/data/vessel_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A877E1CF-47CA-6241-AD0C-8895FBC64180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6BFAE9-C067-AE47-8711-D8D8BBBA95D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" activeTab="2" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" firstSheet="4" activeTab="6" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel size (adipose)" sheetId="2" r:id="rId1"/>
@@ -122,9 +122,6 @@
     <t>Yagihashi, 1978 (7 month-old rats)</t>
   </si>
   <si>
-    <t>Ireland et al., 1977</t>
-  </si>
-  <si>
     <t>Tufto &amp; Rofstad, 1999 (Balb/c nu/nu &amp; D-12 cell)</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>Fernandez-Rodriguez et al., 2016 (C57BL6 &amp; B16F1)</t>
+  </si>
+  <si>
+    <t>Fox et al., 1977</t>
   </si>
 </sst>
 </file>
@@ -768,7 +768,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>53</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>130</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>84.95</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>86.59</v>
@@ -812,7 +812,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>134.80000000000001</v>
@@ -823,7 +823,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>93.3</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>113.1</v>
@@ -855,7 +855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB9AA12-EEBC-1B4E-A018-35116729BAA8}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1020,7 +1020,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>19.45</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>19.13</v>
@@ -1042,7 +1042,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>17.64</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>70.62</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>31.87</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>29.65</v>
@@ -1086,7 +1086,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <v>147.74</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9">
         <v>292.45</v>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10">
         <v>211.93</v>
@@ -1317,8 +1317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8638496-EB20-CE45-9016-2212A07E7085}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B7">
         <v>305</v>

</xml_diff>

<commit_message>
add `Rodrigues et al., 1983` to kidney data
</commit_message>
<xml_diff>
--- a/data/vessel_parameters.xlsx
+++ b/data/vessel_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6BFAE9-C067-AE47-8711-D8D8BBBA95D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C723224-8FF3-5243-87FA-4A712EDBFE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" firstSheet="4" activeTab="6" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
   <si>
     <t>Reference</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>Fox et al., 1977</t>
+  </si>
+  <si>
+    <t>Rodrigues et al., 1983</t>
   </si>
 </sst>
 </file>
@@ -291,8 +294,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{75009760-B3AA-0840-930F-D2CDF2C281B5}" name="Table58" displayName="Table58" ref="A1:E7" totalsRowShown="0">
-  <autoFilter ref="A1:E7" xr:uid="{75009760-B3AA-0840-930F-D2CDF2C281B5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{75009760-B3AA-0840-930F-D2CDF2C281B5}" name="Table58" displayName="Table58" ref="A1:E8" totalsRowShown="0">
+  <autoFilter ref="A1:E8" xr:uid="{75009760-B3AA-0840-930F-D2CDF2C281B5}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{F663CDD2-D3B9-904E-B285-49DAC8870978}" name="Reference"/>
     <tableColumn id="2" xr3:uid="{96EE9805-BA6F-4441-8B97-1F18D839E4E5}" name="Average"/>
@@ -1315,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8638496-EB20-CE45-9016-2212A07E7085}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1434,6 +1437,24 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8">
+        <v>91</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <f>C8/SQRT(D8)</f>
+        <v>0.86602540378443871</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
delete CBM thickness data
</commit_message>
<xml_diff>
--- a/data/vessel_parameters.xlsx
+++ b/data/vessel_parameters.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA51A7E-70B6-F144-9A74-D7F6BF2F18CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A9330C-8F5A-E64B-947F-D44706EA5D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" firstSheet="4" activeTab="4" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" activeTab="3" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel size (adipose)" sheetId="2" r:id="rId1"/>
     <sheet name="Vessel size (tumor)" sheetId="3" r:id="rId2"/>
     <sheet name="Vessel density (adipose)" sheetId="4" r:id="rId3"/>
     <sheet name="Vessel density (tumor)" sheetId="5" r:id="rId4"/>
-    <sheet name="CBM (retina)" sheetId="6" r:id="rId5"/>
-    <sheet name="CBM (muscle)" sheetId="7" r:id="rId6"/>
-    <sheet name="CBM (kidney)" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>Reference</t>
   </si>
@@ -53,9 +50,6 @@
     <t>SE</t>
   </si>
   <si>
-    <t>SD</t>
-  </si>
-  <si>
     <t>Lean_Average</t>
   </si>
   <si>
@@ -80,27 +74,6 @@
     <t>Maquoi et al., 2003</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Cuthbertson &amp; Mandel, 1986</t>
-  </si>
-  <si>
-    <t>Carlson et al., 2003</t>
-  </si>
-  <si>
-    <t>Danis &amp; Yang, 1993</t>
-  </si>
-  <si>
-    <t>Creutzfeldt et al., 1970</t>
-  </si>
-  <si>
-    <t>Lash et al., 1989 (11 wk.)</t>
-  </si>
-  <si>
-    <t>Lash et al., 1989 (18 wk.)</t>
-  </si>
-  <si>
     <t>Lijnen et al., 2007</t>
   </si>
   <si>
@@ -110,18 +83,6 @@
     <t>Lijnen et al., 2003</t>
   </si>
   <si>
-    <t>Chang et al., 2012</t>
-  </si>
-  <si>
-    <t>Gambaro et al., 1992</t>
-  </si>
-  <si>
-    <t>Yagihashi, 1978 (6 month-old rats)</t>
-  </si>
-  <si>
-    <t>Yagihashi, 1978 (7 month-old rats)</t>
-  </si>
-  <si>
     <t>Tufto &amp; Rofstad, 1999 (Balb/c nu/nu &amp; D-12 cell)</t>
   </si>
   <si>
@@ -153,15 +114,6 @@
   </si>
   <si>
     <t>Fernandez-Rodriguez et al., 2016 (C57BL6 &amp; B16F1)</t>
-  </si>
-  <si>
-    <t>Fox et al., 1977</t>
-  </si>
-  <si>
-    <t>Rodrigues et al., 1983</t>
-  </si>
-  <si>
-    <t>Dosso et al., 1990</t>
   </si>
 </sst>
 </file>
@@ -263,48 +215,6 @@
     <tableColumn id="1" xr3:uid="{0F912B10-92FC-BC4D-9A6F-BC8B503601C9}" name="Reference"/>
     <tableColumn id="2" xr3:uid="{06728376-F009-934F-B3F0-B125D2C41224}" name="Average"/>
     <tableColumn id="3" xr3:uid="{A3E965D3-2F22-6744-9E18-FC546CB819AA}" name="SE"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5B52C3C0-4D62-714F-A991-63B550FEAB7D}" name="Table5" displayName="Table5" ref="A1:E5" totalsRowShown="0">
-  <autoFilter ref="A1:E5" xr:uid="{5B52C3C0-4D62-714F-A991-63B550FEAB7D}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{452545DB-0C0F-CB42-AF2A-8F5471D626B0}" name="Reference"/>
-    <tableColumn id="2" xr3:uid="{44232D97-5812-934A-9228-89971953110F}" name="Average"/>
-    <tableColumn id="3" xr3:uid="{E6C561CF-D5E1-3B46-B625-C9845D027517}" name="SD"/>
-    <tableColumn id="4" xr3:uid="{CECE6654-6E54-2947-975A-63F673FBFC15}" name="N"/>
-    <tableColumn id="5" xr3:uid="{61632C65-00B1-FB48-96BC-170EC2D0EAED}" name="SE"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{91BA5396-AA39-234A-8FD8-A94A5EE5E40C}" name="Table6" displayName="Table6" ref="A1:E5" totalsRowShown="0">
-  <autoFilter ref="A1:E5" xr:uid="{91BA5396-AA39-234A-8FD8-A94A5EE5E40C}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{85082DE8-0471-544A-91F8-8FC0E78E56C7}" name="Reference"/>
-    <tableColumn id="2" xr3:uid="{1294BD5A-6719-784F-AB26-9FEA29A99620}" name="Average"/>
-    <tableColumn id="3" xr3:uid="{6E424A94-9406-5642-AD5C-0CBDD4AC95C8}" name="SD"/>
-    <tableColumn id="4" xr3:uid="{6BC8F42A-61E2-AD4B-B9FD-15E2C1CF3327}" name="N"/>
-    <tableColumn id="5" xr3:uid="{4901A108-E9A6-5E40-958F-B53E470CD03B}" name="SE"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{75009760-B3AA-0840-930F-D2CDF2C281B5}" name="Table58" displayName="Table58" ref="A1:E8" totalsRowShown="0">
-  <autoFilter ref="A1:E8" xr:uid="{75009760-B3AA-0840-930F-D2CDF2C281B5}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F663CDD2-D3B9-904E-B285-49DAC8870978}" name="Reference"/>
-    <tableColumn id="2" xr3:uid="{96EE9805-BA6F-4441-8B97-1F18D839E4E5}" name="Average"/>
-    <tableColumn id="3" xr3:uid="{1F3FB073-7DBD-FF4C-B602-EEA5E6607750}" name="SD"/>
-    <tableColumn id="4" xr3:uid="{F5A9B8A8-2E67-A64F-A24E-5EAB6675757E}" name="N"/>
-    <tableColumn id="5" xr3:uid="{88A4B682-E733-934A-8C16-16DEC42C6D52}" name="SE"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -626,21 +536,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>27</v>
@@ -657,7 +567,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>49</v>
@@ -674,7 +584,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>74</v>
@@ -691,7 +601,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>47</v>
@@ -702,7 +612,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>76</v>
@@ -713,7 +623,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>59</v>
@@ -730,7 +640,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <v>108</v>
@@ -774,7 +684,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>53</v>
@@ -785,7 +695,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>130</v>
@@ -796,7 +706,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>84.95</v>
@@ -807,7 +717,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>86.59</v>
@@ -818,7 +728,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>134.80000000000001</v>
@@ -829,7 +739,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>93.3</v>
@@ -840,7 +750,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>113.1</v>
@@ -879,21 +789,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>370</v>
@@ -910,7 +820,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>790</v>
@@ -927,7 +837,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>280</v>
@@ -944,7 +854,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>120</v>
@@ -955,7 +865,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>210</v>
@@ -966,7 +876,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>740</v>
@@ -983,7 +893,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <v>238</v>
@@ -1004,7 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{948AD4BD-5858-C44D-9CCF-6A7A80C70BF7}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1026,7 +936,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>19.45</v>
@@ -1037,7 +947,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>19.13</v>
@@ -1048,7 +958,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>17.64</v>
@@ -1059,7 +969,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>70.62</v>
@@ -1070,7 +980,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>31.87</v>
@@ -1081,7 +991,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>29.65</v>
@@ -1092,7 +1002,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>147.74</v>
@@ -1103,7 +1013,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>292.45</v>
@@ -1114,366 +1024,13 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>211.93</v>
       </c>
       <c r="C10">
         <v>25.6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64CA989-3375-AD42-92AB-E1A53679D5F8}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <v>59</v>
-      </c>
-      <c r="C2">
-        <v>13</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <f>C2/SQRT(D2)</f>
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>92.87</v>
-      </c>
-      <c r="C3">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3" si="0">C3/SQRT(D3)</f>
-        <v>6.6821590822128734</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>89</v>
-      </c>
-      <c r="E4">
-        <f>B4*2.2/100</f>
-        <v>1.9580000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5">
-        <v>93.6</v>
-      </c>
-      <c r="C5">
-        <v>6.12</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <f>C5/SQRT(D5)</f>
-        <v>2.7369472044597427</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3778E71-8C6C-F642-91B5-016CE0E76C01}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2">
-        <v>73</v>
-      </c>
-      <c r="C2">
-        <v>16</v>
-      </c>
-      <c r="D2">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <f>C2/SQRT(D2)</f>
-        <v>5.6568542494923797</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>76.75</v>
-      </c>
-      <c r="C3">
-        <v>14.17</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <f>C3/SQRT(D3)</f>
-        <v>4.4809474444585931</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <v>61.87</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5">
-        <v>55.67</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>1.04</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8638496-EB20-CE45-9016-2212A07E7085}">
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2">
-        <v>178.16</v>
-      </c>
-      <c r="C2">
-        <v>35.61</v>
-      </c>
-      <c r="D2">
-        <v>19</v>
-      </c>
-      <c r="E2">
-        <f>C2/SQRT(D2)</f>
-        <v>8.1694942831307031</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3">
-        <v>224.2</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>27.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4">
-        <v>235.57</v>
-      </c>
-      <c r="E4">
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5">
-        <v>160.5</v>
-      </c>
-      <c r="C5">
-        <v>3.8</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <f>C5/SQRT(D5)</f>
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6">
-        <v>184.6</v>
-      </c>
-      <c r="C6">
-        <v>6.5</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <f>C6/SQRT(D6)</f>
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7">
-        <v>305</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8">
-        <v>91</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>12</v>
-      </c>
-      <c r="E8">
-        <f>C8/SQRT(D8)</f>
-        <v>0.86602540378443871</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add missing data in `Voros et al., 2005` and `Fernandez-Rodriguez et al., 2016`
</commit_message>
<xml_diff>
--- a/data/vessel_parameters.xlsx
+++ b/data/vessel_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A9330C-8F5A-E64B-947F-D44706EA5D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C1A479-0CCD-2844-BD46-32414B657B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" activeTab="3" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel size (adipose)" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>Reference</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Lijnen et al., 2006</t>
   </si>
   <si>
-    <t>Voros et al., 2005</t>
-  </si>
-  <si>
     <t>Maquoi et al., 2003</t>
   </si>
   <si>
@@ -113,17 +110,39 @@
     <t>Mesquita et al., 2012 (Nude &amp; fibrosarcoma)</t>
   </si>
   <si>
-    <t>Fernandez-Rodriguez et al., 2016 (C57BL6 &amp; B16F1)</t>
+    <t>Voros et al., 2005 (7 wk. mice)</t>
+  </si>
+  <si>
+    <t>Voros et al., 2005 (10 wk. mice)</t>
+  </si>
+  <si>
+    <t>Voros et al., 2005 (15 wk. mice)</t>
+  </si>
+  <si>
+    <t>Voros et al., 2005 (Littermate of ob/ob mice)</t>
+  </si>
+  <si>
+    <t>Fernandez-Rodriguez et al., 2016 (Exp 1- C57BL6 &amp; B16F1)</t>
+  </si>
+  <si>
+    <t>Fernandez-Rodriguez et al., 2016 (Exp 2- C57BL6 &amp; B16F1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,8 +168,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -169,8 +189,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9345D645-B0C0-EB46-8246-BA16416A932D}" name="Table1" displayName="Table1" ref="A1:E8" totalsRowShown="0">
-  <autoFilter ref="A1:E8" xr:uid="{9345D645-B0C0-EB46-8246-BA16416A932D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9345D645-B0C0-EB46-8246-BA16416A932D}" name="Table1" displayName="Table1" ref="A1:E10" totalsRowShown="0">
+  <autoFilter ref="A1:E10" xr:uid="{9345D645-B0C0-EB46-8246-BA16416A932D}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B6B21CB4-3BF8-CA4F-B6D1-667B8F16ACAD}" name="Reference"/>
     <tableColumn id="2" xr3:uid="{AD7C98EC-957C-DD40-BE11-28117E12F20A}" name="Lean_Average"/>
@@ -183,8 +203,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{44B5E82D-DA16-C541-862F-3E86577D1164}" name="Table3" displayName="Table3" ref="A1:C8" totalsRowShown="0">
-  <autoFilter ref="A1:C8" xr:uid="{44B5E82D-DA16-C541-862F-3E86577D1164}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{44B5E82D-DA16-C541-862F-3E86577D1164}" name="Table3" displayName="Table3" ref="A1:C10" totalsRowShown="0">
+  <autoFilter ref="A1:C10" xr:uid="{44B5E82D-DA16-C541-862F-3E86577D1164}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A2B929B1-1D90-9E49-83F2-D169F4B69A23}" name="Reference"/>
     <tableColumn id="2" xr3:uid="{D3E2220D-5C65-6942-A58D-E3C127B02764}" name="Average"/>
@@ -195,8 +215,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B76B723-8419-4C40-A482-C96E89DAF113}" name="Table13" displayName="Table13" ref="A1:E8" totalsRowShown="0">
-  <autoFilter ref="A1:E8" xr:uid="{2B76B723-8419-4C40-A482-C96E89DAF113}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B76B723-8419-4C40-A482-C96E89DAF113}" name="Table13" displayName="Table13" ref="A1:E11" totalsRowShown="0">
+  <autoFilter ref="A1:E11" xr:uid="{2B76B723-8419-4C40-A482-C96E89DAF113}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{628F8917-DB36-EB45-9027-3E96F8944A3A}" name="Reference"/>
     <tableColumn id="2" xr3:uid="{6CF8D7DE-ECB1-3141-83D3-8C52A6C13012}" name="Lean_Average"/>
@@ -209,8 +229,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}" name="Table4" displayName="Table4" ref="A1:C10" totalsRowShown="0">
-  <autoFilter ref="A1:C10" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0">
+  <autoFilter ref="A1:C11" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0F912B10-92FC-BC4D-9A6F-BC8B503601C9}" name="Reference"/>
     <tableColumn id="2" xr3:uid="{06728376-F009-934F-B3F0-B125D2C41224}" name="Average"/>
@@ -517,15 +537,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C67B71-C5D5-0C49-8DD9-33AB5A060F17}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
@@ -567,85 +587,119 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B3">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C3">
-        <v>3.4</v>
+        <v>1.9</v>
       </c>
       <c r="D3">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E3">
-        <v>3.3</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B4">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="C4">
-        <v>4.8</v>
+        <v>2.6</v>
       </c>
       <c r="D4">
-        <v>140</v>
+        <v>41</v>
       </c>
       <c r="E4">
-        <v>19</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>49</v>
+      </c>
+      <c r="C5">
+        <v>3.4</v>
       </c>
       <c r="D5">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E5">
-        <v>2.6</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>74</v>
+      </c>
+      <c r="C6">
+        <v>4.8</v>
       </c>
       <c r="D6">
-        <v>76</v>
+        <v>140</v>
       </c>
       <c r="E6">
-        <v>3.9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
-        <v>59</v>
-      </c>
-      <c r="C7">
-        <v>5.0999999999999996</v>
-      </c>
       <c r="D7">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7">
-        <v>2.8</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>76</v>
+      </c>
+      <c r="E8">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="D8">
+      <c r="B9">
+        <v>59</v>
+      </c>
+      <c r="C9">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D9">
+        <v>49</v>
+      </c>
+      <c r="E9">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
         <v>108</v>
       </c>
-      <c r="E8">
+      <c r="E10">
         <v>7.7</v>
       </c>
     </row>
@@ -659,15 +713,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B85283-A6CE-8E41-B263-5F254FE23441}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.1640625" customWidth="1"/>
+    <col min="1" max="1" width="50.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -684,7 +738,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>53</v>
@@ -695,7 +749,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>130</v>
@@ -706,29 +760,29 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4">
-        <v>84.95</v>
+        <v>86.66</v>
       </c>
       <c r="C4">
-        <v>3.75</v>
+        <v>2.7549999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5">
-        <v>86.59</v>
+        <v>88.9</v>
       </c>
       <c r="C5">
-        <v>1.26</v>
+        <v>1.1100000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>134.80000000000001</v>
@@ -739,7 +793,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>93.3</v>
@@ -750,13 +804,35 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>113.1</v>
       </c>
       <c r="C8">
         <v>5.51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>216.46</v>
+      </c>
+      <c r="C9">
+        <v>19.309999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>209.62</v>
+      </c>
+      <c r="C10">
+        <v>15.46</v>
       </c>
     </row>
   </sheetData>
@@ -769,15 +845,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB9AA12-EEBC-1B4E-A018-35116729BAA8}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
@@ -820,85 +896,130 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B3">
+        <v>1200</v>
+      </c>
+      <c r="C3">
+        <v>55</v>
+      </c>
+      <c r="D3">
         <v>790</v>
       </c>
-      <c r="C3">
-        <v>41</v>
-      </c>
-      <c r="D3">
-        <v>490</v>
-      </c>
       <c r="E3">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B4">
-        <v>280</v>
+        <v>850</v>
       </c>
       <c r="C4">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D4">
-        <v>200</v>
+        <v>410</v>
       </c>
       <c r="E4">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>790</v>
+      </c>
+      <c r="C5">
+        <v>41</v>
       </c>
       <c r="D5">
-        <v>120</v>
+        <v>490</v>
       </c>
       <c r="E5">
-        <v>6.2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>210</v>
-      </c>
-      <c r="E6">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>830</v>
+      </c>
+      <c r="C6">
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>740</v>
+        <v>280</v>
       </c>
       <c r="C7">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="D7">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="E7">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>120</v>
+      </c>
+      <c r="E8">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>210</v>
+      </c>
+      <c r="E9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="D8">
+      <c r="B10">
+        <v>740</v>
+      </c>
+      <c r="C10">
+        <v>96</v>
+      </c>
+      <c r="D10">
+        <v>400</v>
+      </c>
+      <c r="E10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
         <v>238</v>
       </c>
-      <c r="E8">
+      <c r="E11">
         <v>16</v>
       </c>
     </row>
@@ -912,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{948AD4BD-5858-C44D-9CCF-6A7A80C70BF7}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -936,7 +1057,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>19.45</v>
@@ -947,7 +1068,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>19.13</v>
@@ -958,7 +1079,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>17.64</v>
@@ -969,7 +1090,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>70.62</v>
@@ -980,56 +1101,67 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B6">
-        <v>31.87</v>
+        <v>48.87</v>
       </c>
       <c r="C6">
-        <v>5.8</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7">
-        <v>29.65</v>
+        <v>31.87</v>
       </c>
       <c r="C7">
-        <v>2.81</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8">
-        <v>147.74</v>
+        <v>29.65</v>
       </c>
       <c r="C8">
-        <v>17.899999999999999</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9">
-        <v>292.45</v>
+        <v>147.74</v>
       </c>
       <c r="C9">
-        <v>28.64</v>
+        <v>17.899999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10">
+        <v>292.45</v>
+      </c>
+      <c r="C10">
+        <v>28.64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
         <v>211.93</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>25.6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edit reference names of `Voros et al., 2005` (mice age -> duration of diet)
</commit_message>
<xml_diff>
--- a/data/vessel_parameters.xlsx
+++ b/data/vessel_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C1A479-0CCD-2844-BD46-32414B657B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC744AD-5496-E74F-B56A-8D8A927DCB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" activeTab="2" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel size (adipose)" sheetId="2" r:id="rId1"/>
@@ -110,15 +110,6 @@
     <t>Mesquita et al., 2012 (Nude &amp; fibrosarcoma)</t>
   </si>
   <si>
-    <t>Voros et al., 2005 (7 wk. mice)</t>
-  </si>
-  <si>
-    <t>Voros et al., 2005 (10 wk. mice)</t>
-  </si>
-  <si>
-    <t>Voros et al., 2005 (15 wk. mice)</t>
-  </si>
-  <si>
     <t>Voros et al., 2005 (Littermate of ob/ob mice)</t>
   </si>
   <si>
@@ -126,6 +117,15 @@
   </si>
   <si>
     <t>Fernandez-Rodriguez et al., 2016 (Exp 2- C57BL6 &amp; B16F1)</t>
+  </si>
+  <si>
+    <t>Voros et al., 2005 (2 wk. diet)</t>
+  </si>
+  <si>
+    <t>Voros et al., 2005 (5 wk. diet)</t>
+  </si>
+  <si>
+    <t>Voros et al., 2005 (15 wk. diet)</t>
   </si>
 </sst>
 </file>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C67B71-C5D5-0C49-8DD9-33AB5A060F17}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,7 +587,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>52</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>50</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>49</v>
@@ -815,7 +815,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <v>216.46</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>209.62</v>
@@ -847,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB9AA12-EEBC-1B4E-A018-35116729BAA8}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,7 +896,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>1200</v>
@@ -913,7 +913,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>850</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>790</v>
@@ -947,7 +947,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>830</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>70.62</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>48.87</v>

</xml_diff>

<commit_message>
add DMSO-treated mice data from `Kostourou et al., 2012`
</commit_message>
<xml_diff>
--- a/data/vessel_parameters.xlsx
+++ b/data/vessel_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC744AD-5496-E74F-B56A-8D8A927DCB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A668201-7C39-6A47-80B4-D416FFBB77A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" activeTab="2" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" firstSheet="1" activeTab="3" xr2:uid="{DAE59B5E-D3EE-024A-92C6-85A458554517}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel size (adipose)" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
   <si>
     <t>Reference</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Voros et al., 2005 (15 wk. diet)</t>
+  </si>
+  <si>
+    <t>Kostourou et al., 2013 (C57BL6/129 &amp; B16F0 cell &amp; DMSO)</t>
   </si>
 </sst>
 </file>
@@ -229,8 +232,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0">
-  <autoFilter ref="A1:C11" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}" name="Table4" displayName="Table4" ref="A1:C12" totalsRowShown="0">
+  <autoFilter ref="A1:C12" xr:uid="{68A2C25F-6C68-A342-93E5-2B5C87963024}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0F912B10-92FC-BC4D-9A6F-BC8B503601C9}" name="Reference"/>
     <tableColumn id="2" xr3:uid="{06728376-F009-934F-B3F0-B125D2C41224}" name="Average"/>
@@ -847,7 +850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB9AA12-EEBC-1B4E-A018-35116729BAA8}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
@@ -1033,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{948AD4BD-5858-C44D-9CCF-6A7A80C70BF7}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1134,34 +1137,45 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B9">
-        <v>147.74</v>
+        <v>64.849999999999994</v>
       </c>
       <c r="C9">
-        <v>17.899999999999999</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10">
-        <v>292.45</v>
+        <v>147.74</v>
       </c>
       <c r="C10">
-        <v>28.64</v>
+        <v>17.899999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>292.45</v>
+      </c>
+      <c r="C11">
+        <v>28.64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>211.93</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>25.6</v>
       </c>
     </row>

</xml_diff>